<commit_message>
modif gestion SSID pour support WPA
</commit_message>
<xml_diff>
--- a/ProjectDocumention/DatasConception.xlsx
+++ b/ProjectDocumention/DatasConception.xlsx
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="181">
   <si>
     <t>IA</t>
   </si>
@@ -723,6 +723,9 @@
   </si>
   <si>
     <t>software interrupt (wheel encoder)</t>
+  </si>
+  <si>
+    <t>power for encoder</t>
   </si>
 </sst>
 </file>
@@ -914,49 +917,49 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2114,10 +2117,10 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L47" sqref="L47"/>
+      <selection pane="bottomRight" activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,13 +2161,13 @@
       <c r="A2" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="33" t="s">
         <v>126</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="21" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2172,11 +2175,11 @@
       <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="33"/>
       <c r="G3" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H3" s="20"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2185,7 +2188,7 @@
       <c r="C4" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="25" t="s">
         <v>156</v>
       </c>
       <c r="E4" s="16"/>
@@ -2206,7 +2209,7 @@
       <c r="C5" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="16"/>
       <c r="F5" s="1">
         <v>1</v>
@@ -2237,7 +2240,7 @@
       <c r="C7" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="20" t="s">
         <v>156</v>
       </c>
       <c r="E7" s="16"/>
@@ -2249,7 +2252,7 @@
       <c r="C8" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="27" t="s">
         <v>155</v>
       </c>
       <c r="E8" s="17"/>
@@ -2261,7 +2264,7 @@
       <c r="C9" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2271,7 +2274,7 @@
       <c r="C10" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="29"/>
       <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2281,7 +2284,7 @@
       <c r="C11" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2292,7 +2295,7 @@
       <c r="C12" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D12" s="25"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2301,7 +2304,7 @@
       <c r="C13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="22" t="s">
         <v>152</v>
       </c>
       <c r="E13" s="15"/>
@@ -2319,7 +2322,7 @@
       <c r="C14" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="15"/>
       <c r="G14" s="11" t="s">
         <v>134</v>
@@ -2344,7 +2347,7 @@
       <c r="A16" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="34" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2352,13 +2355,13 @@
       <c r="A17" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="22"/>
+      <c r="B17" s="34"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="33" t="s">
         <v>128</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -2372,7 +2375,7 @@
       <c r="A19" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="33"/>
       <c r="G19" s="8" t="s">
         <v>134</v>
       </c>
@@ -2384,7 +2387,7 @@
       <c r="A20" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="34" t="s">
         <v>129</v>
       </c>
       <c r="F20" s="1">
@@ -2401,7 +2404,7 @@
       <c r="A21" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="22"/>
+      <c r="B21" s="34"/>
       <c r="F21" s="1">
         <v>4</v>
       </c>
@@ -2416,7 +2419,7 @@
       <c r="A22" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="34" t="s">
         <v>130</v>
       </c>
       <c r="E22" s="14" t="s">
@@ -2436,7 +2439,7 @@
       <c r="A23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="22"/>
+      <c r="B23" s="34"/>
       <c r="E23" s="14" t="s">
         <v>134</v>
       </c>
@@ -2606,7 +2609,7 @@
       <c r="A46" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="30" t="s">
         <v>154</v>
       </c>
       <c r="E46" s="18"/>
@@ -2615,14 +2618,14 @@
       <c r="A47" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="30"/>
+      <c r="D47" s="31"/>
       <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>114</v>
       </c>
-      <c r="D48" s="31"/>
+      <c r="D48" s="32"/>
       <c r="E48" s="18"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -2633,6 +2636,12 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>116</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
started to add  function accross noarow path
</commit_message>
<xml_diff>
--- a/ProjectDocumention/DatasConception.xlsx
+++ b/ProjectDocumention/DatasConception.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="105" windowWidth="23715" windowHeight="9030"/>
+    <workbookView xWindow="5670" yWindow="105" windowWidth="23715" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="ArduinoMegaPin" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>timer 3 a priori utilise par servo</t>
+          <t>timer 3  used by servo
+So servomotor and wheel encoders must be used alternativly</t>
         </r>
       </text>
     </comment>
@@ -826,6 +827,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -851,21 +867,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1241,7 +1242,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G43" sqref="G43:H43"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,13 +1283,13 @@
       <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="26" t="s">
         <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="28" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1296,11 +1297,11 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="26"/>
       <c r="G3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="23"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1309,7 +1310,7 @@
       <c r="C4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="32" t="s">
         <v>112</v>
       </c>
       <c r="E4" s="14"/>
@@ -1330,7 +1331,7 @@
       <c r="C5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="14"/>
       <c r="F5" s="1">
         <v>1</v>
@@ -1373,7 +1374,7 @@
       <c r="C8" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="34" t="s">
         <v>111</v>
       </c>
       <c r="E8" s="15"/>
@@ -1385,7 +1386,7 @@
       <c r="C9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1395,7 +1396,7 @@
       <c r="C10" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="31"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1405,7 +1406,7 @@
       <c r="C11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="30" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1416,7 +1417,7 @@
       <c r="C12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="26"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1425,7 +1426,7 @@
       <c r="C13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="29" t="s">
         <v>108</v>
       </c>
       <c r="E13" s="13"/>
@@ -1443,7 +1444,7 @@
       <c r="C14" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="13"/>
       <c r="G14" s="9" t="s">
         <v>90</v>
@@ -1468,7 +1469,7 @@
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="27" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1476,13 +1477,13 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="27"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="26" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -1496,7 +1497,7 @@
       <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="26"/>
       <c r="G19" s="6" t="s">
         <v>90</v>
       </c>
@@ -1508,7 +1509,7 @@
       <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="27" t="s">
         <v>85</v>
       </c>
       <c r="F20" s="1">
@@ -1525,7 +1526,7 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="36"/>
+      <c r="B21" s="27"/>
       <c r="F21" s="1">
         <v>4</v>
       </c>
@@ -1540,7 +1541,7 @@
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="27" t="s">
         <v>86</v>
       </c>
       <c r="E22" s="12" t="s">
@@ -1560,7 +1561,7 @@
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="36"/>
+      <c r="B23" s="27"/>
       <c r="E23" s="12" t="s">
         <v>90</v>
       </c>
@@ -1739,7 +1740,7 @@
       <c r="A47" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="23" t="s">
         <v>110</v>
       </c>
       <c r="E47" s="16"/>
@@ -1748,14 +1749,14 @@
       <c r="A48" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="33"/>
+      <c r="D48" s="24"/>
       <c r="E48" s="16"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>71</v>
       </c>
-      <c r="D49" s="34"/>
+      <c r="D49" s="25"/>
       <c r="E49" s="16"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1936,17 +1937,17 @@
   </sheetData>
   <autoFilter ref="A1:H72"/>
   <mergeCells count="11">
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D8:D10"/>
     <mergeCell ref="D47:D49"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D8:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2017,10 +2018,10 @@
       <c r="N1" t="s">
         <v>139</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="Q1" s="36"/>
+      <c r="Q1" s="27"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2">

</xml_diff>

<commit_message>
move across narrow path eunder development
</commit_message>
<xml_diff>
--- a/ProjectDocumention/DatasConception.xlsx
+++ b/ProjectDocumention/DatasConception.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="105" windowWidth="23715" windowHeight="9030"/>
+    <workbookView xWindow="6720" yWindow="105" windowWidth="23715" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="ArduinoMegaPin" sheetId="5" r:id="rId1"/>
@@ -44,6 +44,20 @@
         </r>
       </text>
     </comment>
+    <comment ref="D6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>used by delay &amp; millis()</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D8" authorId="0" shapeId="0">
       <text>
         <r>
@@ -55,6 +69,54 @@
             <family val="2"/>
           </rPr>
           <t>used by echoDectection</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>used by PWM 11 &amp; 12</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>used by delay &amp; millis()</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
@@ -187,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="147">
   <si>
     <t>Diametre roue</t>
   </si>
@@ -540,12 +602,6 @@
     <t>I2C</t>
   </si>
   <si>
-    <t>SDA magnetometer</t>
-  </si>
-  <si>
-    <t>SCL magnetometer</t>
-  </si>
-  <si>
     <t>Horn</t>
   </si>
   <si>
@@ -555,12 +611,6 @@
     <t>5v power  read</t>
   </si>
   <si>
-    <t>Left Motor PMW</t>
-  </si>
-  <si>
-    <t>Right Motor PMW</t>
-  </si>
-  <si>
     <t>Left IN1 Motor drive</t>
   </si>
   <si>
@@ -619,6 +669,27 @@
   </si>
   <si>
     <t>PWM</t>
+  </si>
+  <si>
+    <t>SDA &gt;&gt;  BNO Subsytem</t>
+  </si>
+  <si>
+    <t>SCL &gt;&gt; BNO Subsystem</t>
+  </si>
+  <si>
+    <t>15v power read</t>
+  </si>
+  <si>
+    <t>5v power read</t>
+  </si>
+  <si>
+    <t>10v power read</t>
+  </si>
+  <si>
+    <t>Right Motor PWM</t>
+  </si>
+  <si>
+    <t>Left Motor PWM</t>
   </si>
 </sst>
 </file>
@@ -628,7 +699,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -664,8 +735,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -681,12 +765,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,7 +793,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -760,12 +838,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -778,19 +871,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -799,16 +883,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -820,23 +895,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -845,28 +908,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1242,15 +1329,15 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="11.42578125" style="1"/>
-    <col min="5" max="5" width="11.42578125" style="12"/>
+    <col min="5" max="5" width="11.42578125" style="9"/>
     <col min="6" max="7" width="11.42578125" style="1"/>
-    <col min="8" max="8" width="11.42578125" style="11"/>
+    <col min="8" max="8" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1258,7 +1345,7 @@
         <v>79</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>80</v>
@@ -1272,7 +1359,7 @@
       <c r="G1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="11" t="s">
         <v>87</v>
       </c>
       <c r="I1" s="4" t="s">
@@ -1283,13 +1370,13 @@
       <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="19" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1297,11 +1384,11 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="30"/>
       <c r="G3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="28"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1310,18 +1397,18 @@
       <c r="C4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="14"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>134</v>
+      <c r="G4" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1331,19 +1418,19 @@
       <c r="C5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="14"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1353,7 +1440,7 @@
       <c r="D6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1362,42 +1449,46 @@
       <c r="C7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="17"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="34" t="s">
+      <c r="C8" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="17"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="15"/>
+      <c r="C9" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="17"/>
+      <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="15"/>
+      <c r="C10" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="17"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1406,9 +1497,10 @@
       <c r="C11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="20" t="s">
         <v>109</v>
       </c>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1417,7 +1509,8 @@
       <c r="C12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1426,31 +1519,31 @@
       <c r="C13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="G13" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="17"/>
+      <c r="G13" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="13"/>
-      <c r="G14" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>122</v>
+      <c r="D14" s="33"/>
+      <c r="E14" s="17"/>
+      <c r="G14" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1463,13 +1556,13 @@
       <c r="D15" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="31" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1477,19 +1570,19 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="31"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="30" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1497,11 +1590,11 @@
       <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="30"/>
       <c r="G19" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1509,7 +1602,7 @@
       <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="31" t="s">
         <v>85</v>
       </c>
       <c r="F20" s="1">
@@ -1518,33 +1611,33 @@
       <c r="G20" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H20" s="11" t="s">
-        <v>130</v>
+      <c r="H20" s="8" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="27"/>
+      <c r="B21" s="31"/>
       <c r="F21" s="1">
         <v>4</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>132</v>
+      <c r="H21" s="8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F22" s="1">
@@ -1553,16 +1646,16 @@
       <c r="G22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="11" t="s">
-        <v>117</v>
+      <c r="H22" s="8" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="E23" s="12" t="s">
+      <c r="B23" s="31"/>
+      <c r="E23" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F23" s="1">
@@ -1571,8 +1664,8 @@
       <c r="G23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>118</v>
+      <c r="H23" s="8" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1582,8 +1675,8 @@
       <c r="G24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H24" s="11" t="s">
-        <v>131</v>
+      <c r="H24" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1593,8 +1686,8 @@
       <c r="G25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="11" t="s">
-        <v>133</v>
+      <c r="H25" s="8" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1604,8 +1697,8 @@
       <c r="G26" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H26" s="11" t="s">
-        <v>126</v>
+      <c r="H26" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1615,8 +1708,8 @@
       <c r="G27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="11" t="s">
-        <v>127</v>
+      <c r="H27" s="8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1626,8 +1719,8 @@
       <c r="G28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>124</v>
+      <c r="H28" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1637,8 +1730,8 @@
       <c r="G29" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H29" s="11" t="s">
-        <v>125</v>
+      <c r="H29" s="8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1710,14 +1803,14 @@
       <c r="A43" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
       <c r="G43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="H43" s="8" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1740,24 +1833,27 @@
       <c r="A47" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="E47" s="16"/>
+      <c r="E47" s="17"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="24"/>
-      <c r="E48" s="16"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="17"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>71</v>
       </c>
-      <c r="D49" s="25"/>
-      <c r="E49" s="16"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="17"/>
+      <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
@@ -1771,8 +1867,8 @@
       <c r="G51" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H51" s="11" t="s">
-        <v>136</v>
+      <c r="H51" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1782,8 +1878,8 @@
       <c r="G52" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H52" s="11" t="s">
-        <v>119</v>
+      <c r="H52" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1793,7 +1889,7 @@
       <c r="G53" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="H53" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1804,7 +1900,7 @@
       <c r="G54" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="H54" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1815,7 +1911,7 @@
       <c r="G55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H55" s="11" t="s">
+      <c r="H55" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1826,7 +1922,7 @@
       <c r="G56" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H56" s="11" t="s">
+      <c r="H56" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1834,21 +1930,45 @@
       <c r="A57" t="s">
         <v>91</v>
       </c>
+      <c r="G57" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>92</v>
       </c>
+      <c r="G58" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>93</v>
       </c>
+      <c r="G59" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>94</v>
       </c>
+      <c r="G60" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -1877,8 +1997,8 @@
       <c r="G65" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H65" s="11" t="s">
-        <v>128</v>
+      <c r="H65" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -1888,8 +2008,8 @@
       <c r="G66" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H66" s="11" t="s">
-        <v>129</v>
+      <c r="H66" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -1914,8 +2034,8 @@
       <c r="G70" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H70" s="11" t="s">
-        <v>120</v>
+      <c r="H70" s="8" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -1925,8 +2045,8 @@
       <c r="G71" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H71" s="11" t="s">
-        <v>121</v>
+      <c r="H71" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -1937,17 +2057,17 @@
   </sheetData>
   <autoFilter ref="A1:H72"/>
   <mergeCells count="11">
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D8:D10"/>
     <mergeCell ref="D47:D49"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D8:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -1973,9 +2093,9 @@
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.140625" customWidth="1"/>
-    <col min="15" max="15" width="1.42578125" style="20" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" style="19"/>
+    <col min="15" max="15" width="1.42578125" style="14" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
@@ -2010,18 +2130,18 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M1" t="s">
+        <v>134</v>
+      </c>
+      <c r="N1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="N1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q1" s="27"/>
+      <c r="Q1" s="31"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2">
@@ -2071,18 +2191,18 @@
         <f>M2/8</f>
         <v>24.740042147019622</v>
       </c>
-      <c r="P2" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q2" s="19" t="s">
-        <v>141</v>
+      <c r="P2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="P3" s="19">
+      <c r="P3" s="13">
         <v>40</v>
       </c>
-      <c r="Q3" s="21">
+      <c r="Q3" s="15">
         <f>P3*N2/10</f>
         <v>98.960168588078488</v>
       </c>

</xml_diff>

<commit_message>
motors dirved with PID
</commit_message>
<xml_diff>
--- a/ProjectDocumention/DatasConception.xlsx
+++ b/ProjectDocumention/DatasConception.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="105" windowWidth="23715" windowHeight="9030" activeTab="3"/>
+    <workbookView xWindow="6720" yWindow="105" windowWidth="23715" windowHeight="9030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ArduinoMegaPin" sheetId="5" r:id="rId1"/>
@@ -245,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="159">
   <si>
     <t>Diametre roue</t>
   </si>
@@ -719,6 +719,9 @@
   </si>
   <si>
     <t>delta esp8266 relai on off</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -932,21 +935,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -975,6 +963,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1359,13 +1362,13 @@
       <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="35" t="s">
         <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="22" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1373,11 +1376,11 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="35"/>
       <c r="G3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1386,7 +1389,7 @@
       <c r="C4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="27" t="s">
         <v>111</v>
       </c>
       <c r="E4" s="17"/>
@@ -1407,7 +1410,7 @@
       <c r="C5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="17"/>
       <c r="F5" s="1">
         <v>1</v>
@@ -1451,7 +1454,7 @@
       <c r="C8" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="29" t="s">
         <v>110</v>
       </c>
       <c r="E8" s="17"/>
@@ -1464,7 +1467,7 @@
       <c r="C9" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="17"/>
       <c r="G9" s="10"/>
     </row>
@@ -1475,7 +1478,7 @@
       <c r="C10" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="36"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="17"/>
       <c r="G10" s="10"/>
     </row>
@@ -1486,7 +1489,7 @@
       <c r="C11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="25" t="s">
         <v>108</v>
       </c>
       <c r="E11" s="17"/>
@@ -1498,7 +1501,7 @@
       <c r="C12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1508,7 +1511,7 @@
       <c r="C13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="23" t="s">
         <v>107</v>
       </c>
       <c r="E13" s="17"/>
@@ -1526,7 +1529,7 @@
       <c r="C14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="17"/>
       <c r="G14" s="7" t="s">
         <v>89</v>
@@ -1551,7 +1554,7 @@
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="36" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1559,13 +1562,13 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="36"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="35" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -1579,7 +1582,7 @@
       <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="25"/>
+      <c r="B19" s="35"/>
       <c r="G19" s="6" t="s">
         <v>89</v>
       </c>
@@ -1591,7 +1594,7 @@
       <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="36" t="s">
         <v>85</v>
       </c>
       <c r="F20" s="1">
@@ -1608,7 +1611,7 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="26"/>
+      <c r="B21" s="36"/>
       <c r="F21" s="1">
         <v>4</v>
       </c>
@@ -1623,7 +1626,7 @@
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="26"/>
+      <c r="B22" s="36"/>
       <c r="E22" s="9" t="s">
         <v>89</v>
       </c>
@@ -1641,7 +1644,7 @@
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="26"/>
+      <c r="B23" s="36"/>
       <c r="E23" s="9" t="s">
         <v>89</v>
       </c>
@@ -1826,7 +1829,7 @@
       <c r="A47" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="32" t="s">
         <v>109</v>
       </c>
       <c r="E47" s="17"/>
@@ -1836,7 +1839,7 @@
       <c r="A48" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="23"/>
+      <c r="D48" s="33"/>
       <c r="E48" s="17"/>
       <c r="G48" s="10"/>
     </row>
@@ -1844,7 +1847,7 @@
       <c r="A49" t="s">
         <v>71</v>
       </c>
-      <c r="D49" s="24"/>
+      <c r="D49" s="34"/>
       <c r="E49" s="17"/>
       <c r="G49" s="10"/>
     </row>
@@ -2050,17 +2053,17 @@
   </sheetData>
   <autoFilter ref="A1:H72"/>
   <mergeCells count="11">
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D8:D10"/>
     <mergeCell ref="D47:D49"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D8:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2069,10 +2072,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q3"/>
+  <dimension ref="B1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,7 +2094,7 @@
     <col min="17" max="17" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2131,12 +2134,12 @@
       <c r="N1" t="s">
         <v>134</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="26"/>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q1" s="36"/>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>63</v>
       </c>
@@ -2190,8 +2193,11 @@
       <c r="Q2" s="13" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P3" s="13">
         <v>40</v>
       </c>
@@ -2379,7 +2385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Infra red obstabcles detection added
</commit_message>
<xml_diff>
--- a/ProjectDocumention/DatasConception.xlsx
+++ b/ProjectDocumention/DatasConception.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="105" windowWidth="23715" windowHeight="9030" activeTab="4"/>
+    <workbookView xWindow="6720" yWindow="105" windowWidth="23715" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="ArduinoMegaPin" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="mecanique" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ArduinoMegaPin!$A$1:$H$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ArduinoMegaPin!$A$1:$H$71</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -117,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D47" authorId="0">
+    <comment ref="D46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="175">
   <si>
     <t>Diametre roue</t>
   </si>
@@ -744,6 +744,33 @@
   </si>
   <si>
     <t>durcir le positionement des encoders</t>
+  </si>
+  <si>
+    <t>IR detection</t>
+  </si>
+  <si>
+    <t>IR sensors</t>
+  </si>
+  <si>
+    <t>IR sensor</t>
+  </si>
+  <si>
+    <t>1 IR sensor</t>
+  </si>
+  <si>
+    <t>via transistor</t>
+  </si>
+  <si>
+    <t>0 IR sensor</t>
+  </si>
+  <si>
+    <t>2 IR sensor</t>
+  </si>
+  <si>
+    <t>IR sensor power1</t>
+  </si>
+  <si>
+    <t>IR sensor power2</t>
   </si>
 </sst>
 </file>
@@ -902,7 +929,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -941,9 +968,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -960,6 +984,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1005,6 +1038,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Milliers" xfId="3" builtinId="3"/>
@@ -1340,13 +1377,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,13 +1424,13 @@
       <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>82</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="30" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1401,11 +1438,11 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="28"/>
       <c r="G3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="28"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1414,10 +1451,10 @@
       <c r="C4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="E4" s="17"/>
+      <c r="E4" s="16"/>
       <c r="F4" s="1">
         <v>0</v>
       </c>
@@ -1435,15 +1472,15 @@
       <c r="C5" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="17"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="21" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1457,7 +1494,7 @@
       <c r="D6" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1466,23 +1503,23 @@
       <c r="C7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="E7" s="17"/>
+      <c r="E7" s="16"/>
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="17"/>
+      <c r="E8" s="16"/>
       <c r="G8" s="10" t="s">
         <v>89</v>
       </c>
@@ -1494,11 +1531,11 @@
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="38"/>
+      <c r="E9" s="16"/>
       <c r="G9" s="10" t="s">
         <v>89</v>
       </c>
@@ -1510,11 +1547,11 @@
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="16"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1524,10 +1561,10 @@
       <c r="C11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1536,8 +1573,8 @@
       <c r="C12" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1546,10 +1583,10 @@
       <c r="C13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="16"/>
       <c r="G13" s="7" t="s">
         <v>89</v>
       </c>
@@ -1564,8 +1601,8 @@
       <c r="C14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="17"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="16"/>
       <c r="G14" s="7" t="s">
         <v>89</v>
       </c>
@@ -1583,13 +1620,13 @@
       <c r="D15" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="29" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1597,13 +1634,13 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="29"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -1617,7 +1654,7 @@
       <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="28"/>
       <c r="G19" s="6" t="s">
         <v>89</v>
       </c>
@@ -1629,7 +1666,7 @@
       <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="29" t="s">
         <v>85</v>
       </c>
       <c r="F20" s="1">
@@ -1646,7 +1683,7 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="27"/>
+      <c r="B21" s="29"/>
       <c r="F21" s="1">
         <v>4</v>
       </c>
@@ -1661,7 +1698,7 @@
       <c r="A22" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="27"/>
+      <c r="B22" s="29"/>
       <c r="E22" s="9" t="s">
         <v>89</v>
       </c>
@@ -1679,7 +1716,7 @@
       <c r="A23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="27"/>
+      <c r="B23" s="29"/>
       <c r="E23" s="9" t="s">
         <v>89</v>
       </c>
@@ -1763,11 +1800,23 @@
       <c r="A30" t="s">
         <v>53</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1778,36 +1827,78 @@
       <c r="A33" t="s">
         <v>56</v>
       </c>
+      <c r="G33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
+      <c r="G34" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
+      <c r="G35" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>59</v>
       </c>
+      <c r="G36" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="23" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
+      <c r="G37" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>61</v>
       </c>
+      <c r="G38" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>62</v>
       </c>
+      <c r="G39" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="H39" s="23" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1832,90 +1923,86 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="16"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" s="17"/>
+        <v>70</v>
+      </c>
+      <c r="D47" s="26"/>
+      <c r="E47" s="16"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>70</v>
-      </c>
-      <c r="D48" s="24"/>
-      <c r="E48" s="17"/>
+        <v>71</v>
+      </c>
+      <c r="D48" s="27"/>
+      <c r="E48" s="16"/>
       <c r="G48" s="10"/>
     </row>
-    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>71</v>
-      </c>
-      <c r="D49" s="25"/>
-      <c r="E49" s="17"/>
-      <c r="G49" s="10"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>89</v>
@@ -1926,7 +2013,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>89</v>
@@ -1937,7 +2024,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>89</v>
@@ -1948,152 +2035,141 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>90</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>139</v>
+        <v>91</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H57" s="17" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>91</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H58" s="18" t="s">
-        <v>140</v>
+        <v>92</v>
+      </c>
+      <c r="G58" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>92</v>
-      </c>
-      <c r="G59" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H59" s="18" t="s">
-        <v>139</v>
+        <v>93</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H59" s="17" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>93</v>
-      </c>
-      <c r="G60" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H60" s="18" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>99</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H66" s="8" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>104</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H72"/>
+  <autoFilter ref="A1:H71"/>
   <mergeCells count="11">
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="D46:D48"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
@@ -2169,10 +2245,10 @@
       <c r="N1" t="s">
         <v>132</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="Q1" s="27"/>
+      <c r="Q1" s="29"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2">
@@ -2418,10 +2494,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,7 +2506,14 @@
     <col min="5" max="5" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R1" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -2461,8 +2544,23 @@
       <c r="M2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>168</v>
+      </c>
+      <c r="R2" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="T2" s="41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14</v>
       </c>
@@ -2498,8 +2596,25 @@
         <f>L3-B3</f>
         <v>0.17200000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <f>6*Q3</f>
+        <v>0.21599999999999997</v>
+      </c>
+      <c r="Q3">
+        <f>0.18/5</f>
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="R3" s="41">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="S3" s="41">
+        <v>2.4E-2</v>
+      </c>
+      <c r="T3" s="41">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -2531,21 +2646,33 @@
         <f t="shared" ref="J4" si="3">J3*$A$3</f>
         <v>3.1219999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J5" s="20">
+      <c r="P4">
+        <f>Q3*5</f>
+        <v>0.18</v>
+      </c>
+      <c r="Q4">
+        <f>Q3*4</f>
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J5" s="19">
         <f>J4/D4</f>
         <v>0.82592592592592584</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E6" s="21">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E6" s="20">
         <f>2.8/E3</f>
         <v>8.235294117647058</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="R1:T1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2553,7 +2680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>